<commit_message>
Implemented. Using one Linear for Q,K,V across all heads in MHA. It is not any faster :(
</commit_message>
<xml_diff>
--- a/Layers.xlsx
+++ b/Layers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mboedigh\Documents\Julia\Transformers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{DD44C1EC-DA75-49D6-85A9-0388E26B2C46}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{FF644852-889D-4644-AA03-F90F091DD992}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19335" windowHeight="13170" xr2:uid="{62908554-4B77-4B44-93E6-89503C209663}"/>
   </bookViews>
@@ -657,8 +657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9801BA27-C6D7-404F-8CF5-FAC039B2B257}">
   <dimension ref="B1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -666,7 +666,7 @@
     <col min="2" max="2" width="33.140625" customWidth="1"/>
     <col min="3" max="4" width="16.140625" customWidth="1"/>
     <col min="5" max="5" width="16.140625" style="7" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" customWidth="1"/>
+    <col min="6" max="6" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.25">
@@ -690,7 +690,7 @@
         <v>35</v>
       </c>
       <c r="C3" s="25">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
@@ -803,7 +803,7 @@
       </c>
       <c r="E14" s="28">
         <f>n_heads*n_layers*D14</f>
-        <v>96</v>
+        <v>12</v>
       </c>
       <c r="F14" s="27" t="s">
         <v>28</v>
@@ -986,7 +986,7 @@
       </c>
       <c r="E30" s="7">
         <f>n_heads*n_layers*D30</f>
-        <v>96</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
@@ -1046,7 +1046,7 @@
       </c>
       <c r="E36" s="7">
         <f>n_heads*n_layers*D36</f>
-        <v>96</v>
+        <v>12</v>
       </c>
       <c r="F36" t="s">
         <v>4</v>
@@ -1157,7 +1157,7 @@
       </c>
       <c r="E45" s="30">
         <f>SUM(E6:E44)</f>
-        <v>340</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1175,7 +1175,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71E0D1F9-7C59-4E79-88C2-0AA722684F59}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E9AD8450-2DC9-4A4B-9926-4202D956CBAC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://www.boldonjames.com/2008/01/sie/internal/label"/>

</xml_diff>

<commit_message>
changed implementation away from Annotated Transformer and towards "Attention is all you need"
</commit_message>
<xml_diff>
--- a/Layers.xlsx
+++ b/Layers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mboedigh\Documents\Julia\Transformers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{FF644852-889D-4644-AA03-F90F091DD992}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{73471994-CBEA-49A2-BC73-F5D1FBC16921}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19335" windowHeight="13170" xr2:uid="{62908554-4B77-4B44-93E6-89503C209663}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="48">
   <si>
     <t>Step</t>
   </si>
@@ -58,9 +58,6 @@
     <t>Encoder Layer</t>
   </si>
   <si>
-    <t>Encoder SubLayer</t>
-  </si>
-  <si>
     <t>Multi-headed Attn</t>
   </si>
   <si>
@@ -88,9 +85,6 @@
     <t>Decoder Layer</t>
   </si>
   <si>
-    <t>SubLayer</t>
-  </si>
-  <si>
     <t>w1</t>
   </si>
   <si>
@@ -109,9 +103,6 @@
     <t>FeedForward, relu</t>
   </si>
   <si>
-    <t>Param Size</t>
-  </si>
-  <si>
     <t>Q,K,V</t>
   </si>
   <si>
@@ -127,9 +118,6 @@
     <t>Params</t>
   </si>
   <si>
-    <t>quantity</t>
-  </si>
-  <si>
     <t>n params</t>
   </si>
   <si>
@@ -148,9 +136,6 @@
     <t>d_model*d_vocab</t>
   </si>
   <si>
-    <t>d_vocab*d_model</t>
-  </si>
-  <si>
     <t>n_layers</t>
   </si>
   <si>
@@ -161,6 +146,33 @@
   </si>
   <si>
     <t>(d_model*4)*d_model</t>
+  </si>
+  <si>
+    <t>d_vocab</t>
+  </si>
+  <si>
+    <t>head_size</t>
+  </si>
+  <si>
+    <t>diag (gain and bias)</t>
+  </si>
+  <si>
+    <t>SubLayer (mha)</t>
+  </si>
+  <si>
+    <t>SubLayer (self_attn)</t>
+  </si>
+  <si>
+    <t>SubLayer (encoder-attn)</t>
+  </si>
+  <si>
+    <t>SubLayer (FF)</t>
+  </si>
+  <si>
+    <t>Param length</t>
+  </si>
+  <si>
+    <t>param shape (each)</t>
   </si>
 </sst>
 </file>
@@ -255,7 +267,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -281,60 +293,58 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="left" indent="5"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5" applyAlignment="1">
       <alignment horizontal="left" indent="5"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="6" applyAlignment="1">
       <alignment horizontal="left" indent="6"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="6"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="6" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="5" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5" applyAlignment="1">
+      <alignment horizontal="left" indent="6"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
@@ -655,18 +665,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9801BA27-C6D7-404F-8CF5-FAC039B2B257}">
-  <dimension ref="B1:F45"/>
+  <dimension ref="B1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="33.140625" customWidth="1"/>
-    <col min="3" max="4" width="16.140625" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" style="7" customWidth="1"/>
-    <col min="6" max="6" width="23.85546875" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" style="7" customWidth="1"/>
+    <col min="4" max="5" width="16.140625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="23.85546875" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.25">
@@ -674,490 +684,454 @@
         <v>4</v>
       </c>
       <c r="C1" s="7">
-        <v>512</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" s="10">
+        <v>35</v>
+      </c>
+      <c r="C2" s="9">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" s="25">
+        <v>31</v>
+      </c>
+      <c r="C3" s="18">
         <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="7">
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="7">
+        <f>C1/n_heads</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
         <v>0</v>
       </c>
-      <c r="C5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="C7" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="7">
+        <v>1</v>
+      </c>
+      <c r="F9" s="7">
+        <f>C4*C1</f>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="16">
+        <v>2</v>
+      </c>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="20">
+        <v>6</v>
+      </c>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="18">
+        <v>2</v>
+      </c>
+      <c r="E17" s="18"/>
+      <c r="F17" s="22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="11">
+        <v>2</v>
+      </c>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="11">
+        <v>2</v>
+      </c>
+      <c r="E21" s="11"/>
+      <c r="F21" s="23" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="11">
+        <v>2</v>
+      </c>
+      <c r="E22" s="11"/>
+      <c r="F22" s="23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" s="7">
+        <v>1</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="F28" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7" s="7">
-        <v>1</v>
-      </c>
-      <c r="F7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="12"/>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="18"/>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" s="21">
-        <v>2</v>
-      </c>
-      <c r="E12" s="22">
-        <f>D12*n_layers</f>
-        <v>4</v>
-      </c>
-      <c r="F12" s="21" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="27">
-        <v>6</v>
-      </c>
-      <c r="E14" s="28">
-        <f>n_heads*n_layers*D14</f>
-        <v>12</v>
-      </c>
-      <c r="F14" s="27" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="D15" s="24">
-        <v>2</v>
-      </c>
-      <c r="E15" s="25">
-        <f>D15*n_layers</f>
-        <v>4</v>
-      </c>
-      <c r="F15" s="31" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="24"/>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="12"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" s="12">
-        <v>2</v>
-      </c>
-      <c r="E18" s="13">
-        <f>D18*n_layers</f>
-        <v>4</v>
-      </c>
-      <c r="F18" s="12"/>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D19" s="12">
-        <v>2</v>
-      </c>
-      <c r="E19" s="13">
-        <f>D19*n_layers</f>
-        <v>4</v>
-      </c>
-      <c r="F19" s="32" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="D20" s="12">
-        <v>2</v>
-      </c>
-      <c r="E20" s="13">
-        <f>D20*n_layers</f>
-        <v>4</v>
-      </c>
-      <c r="F20" s="32" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="12"/>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C23" t="s">
-        <v>3</v>
-      </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-      <c r="E23" s="7">
-        <v>1</v>
-      </c>
-      <c r="F23" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F24" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F25" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C28" t="s">
-        <v>34</v>
-      </c>
-      <c r="D28">
-        <v>2</v>
-      </c>
-      <c r="E28" s="7">
-        <f>D12*n_layers</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C30" t="s">
-        <v>27</v>
-      </c>
-      <c r="D30">
-        <v>6</v>
-      </c>
-      <c r="E30" s="7">
-        <f>n_heads*n_layers*D30</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C31" t="s">
-        <v>3</v>
-      </c>
-      <c r="D31">
-        <v>2</v>
-      </c>
-      <c r="E31" s="7">
-        <f>D31*n_layers</f>
-        <v>4</v>
+      <c r="D31" s="7">
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D33" s="7">
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B34" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C34" t="s">
-        <v>34</v>
-      </c>
-      <c r="D34">
-        <v>2</v>
-      </c>
-      <c r="E34" s="7">
-        <f>D34*n_layers</f>
-        <v>4</v>
+      <c r="B34" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D34" s="7">
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B37" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C36" t="s">
-        <v>27</v>
-      </c>
-      <c r="D36">
-        <v>6</v>
-      </c>
-      <c r="E36" s="7">
-        <f>n_heads*n_layers*D36</f>
-        <v>12</v>
-      </c>
-      <c r="F36" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B37" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C37" t="s">
-        <v>3</v>
-      </c>
-      <c r="D37">
-        <v>2</v>
-      </c>
-      <c r="E37" s="7">
-        <f>D37*n_layers</f>
-        <v>4</v>
+      <c r="C37" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D37" s="7">
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B39" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D39" s="7">
         <v>6</v>
       </c>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B39" s="3" t="s">
-        <v>19</v>
+      <c r="F39" s="7" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B40" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C40" t="s">
-        <v>34</v>
-      </c>
-      <c r="D40">
-        <v>2</v>
-      </c>
-      <c r="E40" s="7">
-        <f>D40*n_layers</f>
-        <v>4</v>
+      <c r="B40" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D40" s="7">
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B41" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C41" t="s">
-        <v>20</v>
-      </c>
-      <c r="D41">
-        <v>2</v>
-      </c>
-      <c r="E41" s="7">
-        <f>D41*n_layers</f>
-        <v>4</v>
-      </c>
-      <c r="F41" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B42" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C42" t="s">
-        <v>21</v>
-      </c>
-      <c r="D42">
-        <v>2</v>
-      </c>
-      <c r="E42" s="7">
-        <f>D42*n_layers</f>
-        <v>4</v>
-      </c>
-      <c r="F42" t="s">
-        <v>22</v>
+      <c r="B42" s="3" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B43" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D43" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B44" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D44" s="7">
+        <v>2</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B45" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D45" s="7">
+        <v>2</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B46" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
-        <v>37</v>
-      </c>
-      <c r="C44" t="s">
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B47" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>33</v>
+      </c>
+      <c r="C48" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D44">
-        <v>2</v>
-      </c>
-      <c r="E44" s="7">
-        <f>D44</f>
-        <v>2</v>
-      </c>
-      <c r="F44" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B45" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="E45" s="30">
-        <f>SUM(E6:E44)</f>
-        <v>88</v>
+      <c r="D48" s="7">
+        <v>2</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B49" s="21" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1175,7 +1149,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E9AD8450-2DC9-4A4B-9926-4202D956CBAC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F7C5F53-3470-4A2A-98EF-948CD2EEFA2D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://www.boldonjames.com/2008/01/sie/internal/label"/>

</xml_diff>

<commit_message>
Successfully trained stutter task while using 6 layers.
</commit_message>
<xml_diff>
--- a/Layers.xlsx
+++ b/Layers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mboedigh\Documents\Julia\Transformers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0890D34E-3671-416A-87AA-16EC3E2B7B38}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B029CC25-3E2C-4DE3-AE78-54BAE5BF2898}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19335" windowHeight="13170" xr2:uid="{62908554-4B77-4B44-93E6-89503C209663}"/>
   </bookViews>
@@ -227,13 +227,17 @@
     <t>param no.</t>
   </si>
   <si>
-    <t>Enter number of layer (must not exeed n_layers)</t>
+    <t>Enter number of layer in orange square below (must not exeed n_layers)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -328,7 +332,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -336,8 +340,9 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -368,13 +373,17 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="6"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="8">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
     <cellStyle name="20% - Accent3" xfId="4" builtinId="38"/>
     <cellStyle name="40% - Accent1" xfId="2" builtinId="31"/>
     <cellStyle name="60% - Accent1" xfId="3" builtinId="32"/>
     <cellStyle name="60% - Accent3" xfId="5" builtinId="40"/>
+    <cellStyle name="Comma" xfId="7" builtinId="3"/>
     <cellStyle name="Input" xfId="6" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -691,8 +700,8 @@
   <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G59" sqref="G59"/>
+      <pane ySplit="5" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I61" sqref="I61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -709,7 +718,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="1">
-        <v>512</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -727,7 +736,7 @@
         <v>4</v>
       </c>
       <c r="D3" s="5">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
@@ -746,7 +755,7 @@
       </c>
       <c r="D5" s="1">
         <f>D1/n_heads</f>
-        <v>64</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -795,11 +804,11 @@
       </c>
       <c r="G8" s="1">
         <f>d_model*d_vocab</f>
-        <v>6656</v>
+        <v>832</v>
       </c>
       <c r="H8" s="1">
         <f>G8*F8</f>
-        <v>6656</v>
+        <v>832</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -823,11 +832,11 @@
       </c>
       <c r="G9" s="1">
         <f>d_model*d_head*n_heads</f>
-        <v>262144</v>
+        <v>4096</v>
       </c>
       <c r="H9" s="1">
         <f t="shared" ref="H9:H52" si="1">G9*F9</f>
-        <v>1572864</v>
+        <v>24576</v>
       </c>
       <c r="I9" s="7" t="s">
         <v>20</v>
@@ -854,11 +863,11 @@
       </c>
       <c r="G10" s="1">
         <f>d_head*n_heads</f>
-        <v>512</v>
+        <v>64</v>
       </c>
       <c r="H10" s="1">
         <f t="shared" si="1"/>
-        <v>3072</v>
+        <v>384</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -882,11 +891,11 @@
       </c>
       <c r="G11" s="1">
         <f>d_model*d_head*n_heads</f>
-        <v>262144</v>
+        <v>4096</v>
       </c>
       <c r="H11" s="1">
         <f t="shared" si="1"/>
-        <v>1572864</v>
+        <v>24576</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -910,11 +919,11 @@
       </c>
       <c r="G12" s="1">
         <f>d_head*n_heads</f>
-        <v>512</v>
+        <v>64</v>
       </c>
       <c r="H12" s="1">
         <f t="shared" si="1"/>
-        <v>3072</v>
+        <v>384</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -938,11 +947,11 @@
       </c>
       <c r="G13" s="1">
         <f>d_model*d_head*n_heads</f>
-        <v>262144</v>
+        <v>4096</v>
       </c>
       <c r="H13" s="1">
         <f t="shared" si="1"/>
-        <v>1572864</v>
+        <v>24576</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -966,11 +975,11 @@
       </c>
       <c r="G14" s="1">
         <f>d_head*n_heads</f>
-        <v>512</v>
+        <v>64</v>
       </c>
       <c r="H14" s="1">
         <f t="shared" si="1"/>
-        <v>3072</v>
+        <v>384</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -994,11 +1003,11 @@
       </c>
       <c r="G15" s="1">
         <f>d_model*d_head*n_heads</f>
-        <v>262144</v>
+        <v>4096</v>
       </c>
       <c r="H15" s="1">
         <f t="shared" si="1"/>
-        <v>1572864</v>
+        <v>24576</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1022,11 +1031,11 @@
       </c>
       <c r="G16" s="4">
         <f>n_heads*d_head</f>
-        <v>512</v>
+        <v>64</v>
       </c>
       <c r="H16" s="1">
         <f t="shared" si="1"/>
-        <v>3072</v>
+        <v>384</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1050,11 +1059,11 @@
       </c>
       <c r="G17" s="1">
         <f>d_model</f>
-        <v>512</v>
+        <v>64</v>
       </c>
       <c r="H17" s="1">
         <f>G17*F17</f>
-        <v>3072</v>
+        <v>384</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1078,11 +1087,11 @@
       </c>
       <c r="G18" s="1">
         <f>d_model</f>
-        <v>512</v>
+        <v>64</v>
       </c>
       <c r="H18" s="1">
         <f>G18*F18</f>
-        <v>3072</v>
+        <v>384</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1106,11 +1115,11 @@
       </c>
       <c r="G19" s="1">
         <f>d_model*(d_model*4)</f>
-        <v>1048576</v>
+        <v>16384</v>
       </c>
       <c r="H19" s="1">
         <f t="shared" si="1"/>
-        <v>6291456</v>
+        <v>98304</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1134,11 +1143,11 @@
       </c>
       <c r="G20" s="1">
         <f>(d_model*4)</f>
-        <v>2048</v>
+        <v>256</v>
       </c>
       <c r="H20" s="1">
         <f t="shared" si="1"/>
-        <v>12288</v>
+        <v>1536</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1162,11 +1171,11 @@
       </c>
       <c r="G21" s="1">
         <f>d_model*4*d_model</f>
-        <v>1048576</v>
+        <v>16384</v>
       </c>
       <c r="H21" s="1">
         <f t="shared" si="1"/>
-        <v>6291456</v>
+        <v>98304</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1190,11 +1199,11 @@
       </c>
       <c r="G22" s="4">
         <f>d_model</f>
-        <v>512</v>
+        <v>64</v>
       </c>
       <c r="H22" s="1">
         <f t="shared" si="1"/>
-        <v>3072</v>
+        <v>384</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1218,11 +1227,11 @@
       </c>
       <c r="G23" s="1">
         <f>d_model</f>
-        <v>512</v>
+        <v>64</v>
       </c>
       <c r="H23" s="1">
         <f>G23*F23</f>
-        <v>3072</v>
+        <v>384</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1246,11 +1255,11 @@
       </c>
       <c r="G24" s="1">
         <f>d_model</f>
-        <v>512</v>
+        <v>64</v>
       </c>
       <c r="H24" s="1">
         <f>G24*F24</f>
-        <v>3072</v>
+        <v>384</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1274,11 +1283,11 @@
       </c>
       <c r="G25" s="1">
         <f>d_model*d_head*n_heads</f>
-        <v>262144</v>
+        <v>4096</v>
       </c>
       <c r="H25" s="1">
         <f t="shared" si="1"/>
-        <v>1572864</v>
+        <v>24576</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1302,11 +1311,11 @@
       </c>
       <c r="G26" s="1">
         <f>d_head*n_heads</f>
-        <v>512</v>
+        <v>64</v>
       </c>
       <c r="H26" s="1">
         <f t="shared" si="1"/>
-        <v>3072</v>
+        <v>384</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1330,11 +1339,11 @@
       </c>
       <c r="G27" s="1">
         <f>d_model*d_head*n_heads</f>
-        <v>262144</v>
+        <v>4096</v>
       </c>
       <c r="H27" s="1">
         <f t="shared" si="1"/>
-        <v>1572864</v>
+        <v>24576</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -1358,11 +1367,11 @@
       </c>
       <c r="G28" s="1">
         <f>d_head*n_heads</f>
-        <v>512</v>
+        <v>64</v>
       </c>
       <c r="H28" s="1">
         <f t="shared" si="1"/>
-        <v>3072</v>
+        <v>384</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -1386,11 +1395,11 @@
       </c>
       <c r="G29" s="1">
         <f>d_model*d_head*n_heads</f>
-        <v>262144</v>
+        <v>4096</v>
       </c>
       <c r="H29" s="1">
         <f t="shared" si="1"/>
-        <v>1572864</v>
+        <v>24576</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -1414,11 +1423,11 @@
       </c>
       <c r="G30" s="1">
         <f>d_head*n_heads</f>
-        <v>512</v>
+        <v>64</v>
       </c>
       <c r="H30" s="1">
         <f t="shared" si="1"/>
-        <v>3072</v>
+        <v>384</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -1442,11 +1451,11 @@
       </c>
       <c r="G31" s="1">
         <f>d_model*d_head*n_heads</f>
-        <v>262144</v>
+        <v>4096</v>
       </c>
       <c r="H31" s="1">
         <f t="shared" si="1"/>
-        <v>1572864</v>
+        <v>24576</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -1470,11 +1479,11 @@
       </c>
       <c r="G32" s="4">
         <f>n_heads*d_head</f>
-        <v>512</v>
+        <v>64</v>
       </c>
       <c r="H32" s="1">
         <f t="shared" si="1"/>
-        <v>3072</v>
+        <v>384</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -1498,11 +1507,11 @@
       </c>
       <c r="G33" s="1">
         <f>d_model</f>
-        <v>512</v>
+        <v>64</v>
       </c>
       <c r="H33" s="1">
         <f>G33*F33</f>
-        <v>3072</v>
+        <v>384</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -1526,11 +1535,11 @@
       </c>
       <c r="G34" s="1">
         <f>d_model</f>
-        <v>512</v>
+        <v>64</v>
       </c>
       <c r="H34" s="1">
         <f>G34*F34</f>
-        <v>3072</v>
+        <v>384</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -1554,11 +1563,11 @@
       </c>
       <c r="G35" s="1">
         <f>d_model*d_head*n_heads</f>
-        <v>262144</v>
+        <v>4096</v>
       </c>
       <c r="H35" s="1">
         <f t="shared" si="1"/>
-        <v>1572864</v>
+        <v>24576</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -1582,11 +1591,11 @@
       </c>
       <c r="G36" s="1">
         <f>d_head*n_heads</f>
-        <v>512</v>
+        <v>64</v>
       </c>
       <c r="H36" s="1">
         <f t="shared" si="1"/>
-        <v>3072</v>
+        <v>384</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -1610,11 +1619,11 @@
       </c>
       <c r="G37" s="1">
         <f>d_model*d_head*n_heads</f>
-        <v>262144</v>
+        <v>4096</v>
       </c>
       <c r="H37" s="1">
         <f t="shared" si="1"/>
-        <v>1572864</v>
+        <v>24576</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -1638,11 +1647,11 @@
       </c>
       <c r="G38" s="1">
         <f>d_head*n_heads</f>
-        <v>512</v>
+        <v>64</v>
       </c>
       <c r="H38" s="1">
         <f t="shared" si="1"/>
-        <v>3072</v>
+        <v>384</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -1666,11 +1675,11 @@
       </c>
       <c r="G39" s="1">
         <f>d_model*d_head*n_heads</f>
-        <v>262144</v>
+        <v>4096</v>
       </c>
       <c r="H39" s="1">
         <f t="shared" si="1"/>
-        <v>1572864</v>
+        <v>24576</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -1694,11 +1703,11 @@
       </c>
       <c r="G40" s="1">
         <f>d_head*n_heads</f>
-        <v>512</v>
+        <v>64</v>
       </c>
       <c r="H40" s="1">
         <f t="shared" si="1"/>
-        <v>3072</v>
+        <v>384</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -1722,11 +1731,11 @@
       </c>
       <c r="G41" s="1">
         <f>d_model*d_head*n_heads</f>
-        <v>262144</v>
+        <v>4096</v>
       </c>
       <c r="H41" s="1">
         <f t="shared" si="1"/>
-        <v>1572864</v>
+        <v>24576</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -1750,11 +1759,11 @@
       </c>
       <c r="G42" s="4">
         <f>n_heads*d_head</f>
-        <v>512</v>
+        <v>64</v>
       </c>
       <c r="H42" s="1">
         <f t="shared" si="1"/>
-        <v>3072</v>
+        <v>384</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -1778,11 +1787,11 @@
       </c>
       <c r="G43" s="1">
         <f>d_model</f>
-        <v>512</v>
+        <v>64</v>
       </c>
       <c r="H43" s="1">
         <f>G43*F43</f>
-        <v>3072</v>
+        <v>384</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -1806,11 +1815,11 @@
       </c>
       <c r="G44" s="1">
         <f>d_model</f>
-        <v>512</v>
+        <v>64</v>
       </c>
       <c r="H44" s="1">
         <f>G44*F44</f>
-        <v>3072</v>
+        <v>384</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -1834,11 +1843,11 @@
       </c>
       <c r="G45" s="1">
         <f>d_model*(d_model*4)</f>
-        <v>1048576</v>
+        <v>16384</v>
       </c>
       <c r="H45" s="1">
         <f t="shared" si="1"/>
-        <v>6291456</v>
+        <v>98304</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -1862,11 +1871,11 @@
       </c>
       <c r="G46" s="1">
         <f>(d_model*4)</f>
-        <v>2048</v>
+        <v>256</v>
       </c>
       <c r="H46" s="1">
         <f t="shared" si="1"/>
-        <v>12288</v>
+        <v>1536</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -1890,11 +1899,11 @@
       </c>
       <c r="G47" s="1">
         <f>d_model*4*d_model</f>
-        <v>1048576</v>
+        <v>16384</v>
       </c>
       <c r="H47" s="1">
         <f t="shared" si="1"/>
-        <v>6291456</v>
+        <v>98304</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -1918,11 +1927,11 @@
       </c>
       <c r="G48" s="4">
         <f>d_model</f>
-        <v>512</v>
+        <v>64</v>
       </c>
       <c r="H48" s="1">
         <f t="shared" si="1"/>
-        <v>3072</v>
+        <v>384</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
@@ -1946,11 +1955,11 @@
       </c>
       <c r="G49" s="1">
         <f>d_model</f>
-        <v>512</v>
+        <v>64</v>
       </c>
       <c r="H49" s="1">
         <f>G49*F49</f>
-        <v>3072</v>
+        <v>384</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -1974,11 +1983,11 @@
       </c>
       <c r="G50" s="1">
         <f>d_model</f>
-        <v>512</v>
+        <v>64</v>
       </c>
       <c r="H50" s="1">
         <f>G50*F50</f>
-        <v>3072</v>
+        <v>384</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -1997,11 +2006,11 @@
       </c>
       <c r="G51" s="1">
         <f>d_model*d_vocab</f>
-        <v>6656</v>
+        <v>832</v>
       </c>
       <c r="H51" s="1">
         <f t="shared" si="1"/>
-        <v>6656</v>
+        <v>832</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -2037,11 +2046,11 @@
       </c>
       <c r="G53" s="1">
         <f>SUM(G8:G52)</f>
-        <v>7369741</v>
-      </c>
-      <c r="H53" s="1">
+        <v>118413</v>
+      </c>
+      <c r="H53" s="12">
         <f>SUM(H8:H52)</f>
-        <v>44151821</v>
+        <v>702093</v>
       </c>
     </row>
   </sheetData>
@@ -2059,7 +2068,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7EA68EE-A4DC-4837-959A-B674DA2AD51D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E649360-7EF8-4F2B-B1A5-DEB98B446B5D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://www.boldonjames.com/2008/01/sie/internal/label"/>

</xml_diff>